<commit_message>
annotate the control treatments
</commit_message>
<xml_diff>
--- a/3-Doc/Info File_FrostSeededBrassicas_Musgrave 2022, Field E4.xlsx
+++ b/3-Doc/Info File_FrostSeededBrassicas_Musgrave 2022, Field E4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hn337/Documents/Frost-seeded-brassica/3-Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BE8E86-B0F8-3447-8257-EE9D2302B8CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F9826D-4C65-E143-990D-0DD047227D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50880" yWindow="1880" windowWidth="25640" windowHeight="12320" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50880" yWindow="1880" windowWidth="25640" windowHeight="16820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AerialPhoto" sheetId="1" r:id="rId1"/>
@@ -816,7 +816,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -863,6 +863,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor theme="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1047,7 +1053,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1137,9 +1143,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1405,6 +1408,37 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1880,7 +1914,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="6" spans="1:1" ht="20">
-      <c r="A6" s="133" t="s">
+      <c r="A6" s="132" t="s">
         <v>206</v>
       </c>
     </row>
@@ -1901,7 +1935,9 @@
   </sheetPr>
   <dimension ref="A1:Z58"/>
   <sheetViews>
-    <sheetView topLeftCell="D7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O45" sqref="O45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -1914,26 +1950,26 @@
     <row r="1" spans="1:26" ht="18">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
-      <c r="I1" s="135"/>
-      <c r="J1" s="135"/>
-      <c r="K1" s="135"/>
-      <c r="L1" s="135"/>
-      <c r="M1" s="135"/>
-      <c r="N1" s="135"/>
-      <c r="O1" s="135"/>
-      <c r="P1" s="135"/>
-      <c r="Q1" s="135"/>
-      <c r="R1" s="135"/>
-      <c r="S1" s="135"/>
-      <c r="T1" s="135"/>
-      <c r="U1" s="135"/>
-      <c r="V1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="134"/>
+      <c r="I1" s="134"/>
+      <c r="J1" s="134"/>
+      <c r="K1" s="134"/>
+      <c r="L1" s="134"/>
+      <c r="M1" s="134"/>
+      <c r="N1" s="134"/>
+      <c r="O1" s="134"/>
+      <c r="P1" s="134"/>
+      <c r="Q1" s="134"/>
+      <c r="R1" s="134"/>
+      <c r="S1" s="134"/>
+      <c r="T1" s="134"/>
+      <c r="U1" s="134"/>
+      <c r="V1" s="134"/>
       <c r="W1" s="2"/>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
@@ -1968,31 +2004,31 @@
     <row r="3" spans="1:26" ht="15">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="137" t="s">
+      <c r="C3" s="136" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="138"/>
-      <c r="E3" s="138"/>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
-      <c r="H3" s="138"/>
-      <c r="I3" s="138"/>
-      <c r="J3" s="138"/>
-      <c r="K3" s="138"/>
-      <c r="L3" s="138"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
+      <c r="F3" s="137"/>
+      <c r="G3" s="137"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="137"/>
+      <c r="J3" s="137"/>
+      <c r="K3" s="137"/>
+      <c r="L3" s="137"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="137" t="s">
+      <c r="N3" s="136" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="138"/>
-      <c r="P3" s="138"/>
-      <c r="Q3" s="138"/>
-      <c r="R3" s="138"/>
-      <c r="S3" s="138"/>
-      <c r="T3" s="138"/>
-      <c r="U3" s="138"/>
-      <c r="V3" s="138"/>
-      <c r="W3" s="138"/>
+      <c r="O3" s="137"/>
+      <c r="P3" s="137"/>
+      <c r="Q3" s="137"/>
+      <c r="R3" s="137"/>
+      <c r="S3" s="137"/>
+      <c r="T3" s="137"/>
+      <c r="U3" s="137"/>
+      <c r="V3" s="137"/>
+      <c r="W3" s="137"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
     </row>
@@ -2069,16 +2105,16 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="1:26" ht="16">
-      <c r="A5" s="139" t="s">
+      <c r="A5" s="138" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="139" t="s">
+      <c r="B5" s="138" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="148" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="12" t="s">
@@ -2133,12 +2169,12 @@
       <c r="Z5" s="22"/>
     </row>
     <row r="6" spans="1:26" ht="57">
-      <c r="A6" s="140"/>
-      <c r="B6" s="140"/>
+      <c r="A6" s="139"/>
+      <c r="B6" s="139"/>
       <c r="C6" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="149" t="s">
         <v>18</v>
       </c>
       <c r="E6" s="25" t="s">
@@ -2205,10 +2241,10 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="18">
-      <c r="A7" s="140"/>
-      <c r="B7" s="140"/>
+      <c r="A7" s="139"/>
+      <c r="B7" s="139"/>
       <c r="C7" s="23"/>
-      <c r="D7" s="24"/>
+      <c r="D7" s="149"/>
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
@@ -2233,10 +2269,10 @@
       <c r="Z7" s="35"/>
     </row>
     <row r="8" spans="1:26" ht="18">
-      <c r="A8" s="140"/>
-      <c r="B8" s="140"/>
+      <c r="A8" s="139"/>
+      <c r="B8" s="139"/>
       <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
+      <c r="D8" s="149"/>
       <c r="E8" s="25"/>
       <c r="F8" s="25"/>
       <c r="G8" s="25"/>
@@ -2261,28 +2297,28 @@
       <c r="Z8" s="35"/>
     </row>
     <row r="9" spans="1:26" ht="18">
-      <c r="A9" s="141"/>
-      <c r="B9" s="140"/>
+      <c r="A9" s="140"/>
+      <c r="B9" s="139"/>
       <c r="C9" s="36"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="41"/>
+      <c r="D9" s="150"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="40"/>
       <c r="L9" s="27"/>
       <c r="M9" s="28"/>
-      <c r="N9" s="42"/>
-      <c r="O9" s="43"/>
-      <c r="P9" s="44"/>
-      <c r="Q9" s="44"/>
-      <c r="R9" s="44"/>
-      <c r="S9" s="44"/>
-      <c r="T9" s="44"/>
-      <c r="U9" s="44"/>
-      <c r="V9" s="45"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="43"/>
+      <c r="Q9" s="43"/>
+      <c r="R9" s="43"/>
+      <c r="S9" s="43"/>
+      <c r="T9" s="43"/>
+      <c r="U9" s="43"/>
+      <c r="V9" s="44"/>
       <c r="W9" s="33"/>
       <c r="X9" s="33"/>
       <c r="Y9" s="34"/>
@@ -2290,7 +2326,7 @@
     </row>
     <row r="10" spans="1:26" ht="19">
       <c r="A10" s="1"/>
-      <c r="B10" s="140"/>
+      <c r="B10" s="139"/>
       <c r="C10" s="23" t="s">
         <v>36</v>
       </c>
@@ -2303,13 +2339,13 @@
       <c r="F10" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="25" t="s">
+      <c r="G10" s="154" t="s">
         <v>37</v>
       </c>
       <c r="H10" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="I10" s="23" t="s">
+      <c r="I10" s="151" t="s">
         <v>12</v>
       </c>
       <c r="J10" s="24" t="s">
@@ -2350,7 +2386,7 @@
     </row>
     <row r="11" spans="1:26" ht="57">
       <c r="A11" s="1"/>
-      <c r="B11" s="140"/>
+      <c r="B11" s="139"/>
       <c r="C11" s="23" t="s">
         <v>39</v>
       </c>
@@ -2363,13 +2399,13 @@
       <c r="F11" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="G11" s="154" t="s">
         <v>18</v>
       </c>
       <c r="H11" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="I11" s="23" t="s">
+      <c r="I11" s="151" t="s">
         <v>41</v>
       </c>
       <c r="J11" s="24" t="s">
@@ -2399,7 +2435,7 @@
       <c r="T11" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="U11" s="46" t="s">
+      <c r="U11" s="45" t="s">
         <v>24</v>
       </c>
       <c r="V11" s="32"/>
@@ -2410,26 +2446,26 @@
     </row>
     <row r="12" spans="1:26" ht="18">
       <c r="A12" s="1"/>
-      <c r="B12" s="140"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="48"/>
+      <c r="B12" s="139"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="155"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="152"/>
+      <c r="J12" s="47"/>
       <c r="K12" s="32"/>
       <c r="L12" s="34"/>
       <c r="M12" s="33"/>
-      <c r="N12" s="50"/>
+      <c r="N12" s="49"/>
       <c r="O12" s="33"/>
-      <c r="P12" s="46"/>
-      <c r="Q12" s="46"/>
-      <c r="R12" s="46"/>
-      <c r="S12" s="46"/>
-      <c r="T12" s="46"/>
-      <c r="U12" s="46"/>
+      <c r="P12" s="45"/>
+      <c r="Q12" s="45"/>
+      <c r="R12" s="45"/>
+      <c r="S12" s="45"/>
+      <c r="T12" s="45"/>
+      <c r="U12" s="45"/>
       <c r="V12" s="32"/>
       <c r="W12" s="33"/>
       <c r="X12" s="33"/>
@@ -2438,26 +2474,26 @@
     </row>
     <row r="13" spans="1:26" ht="18">
       <c r="A13" s="1"/>
-      <c r="B13" s="140"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="48"/>
+      <c r="B13" s="139"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="155"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="152"/>
+      <c r="J13" s="47"/>
       <c r="K13" s="32"/>
       <c r="L13" s="34"/>
       <c r="M13" s="33"/>
-      <c r="N13" s="50"/>
+      <c r="N13" s="49"/>
       <c r="O13" s="33"/>
-      <c r="P13" s="46"/>
-      <c r="Q13" s="46"/>
-      <c r="R13" s="46"/>
-      <c r="S13" s="46"/>
-      <c r="T13" s="46"/>
-      <c r="U13" s="46"/>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="45"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="45"/>
+      <c r="T13" s="45"/>
+      <c r="U13" s="45"/>
       <c r="V13" s="32"/>
       <c r="W13" s="33"/>
       <c r="X13" s="33"/>
@@ -2466,343 +2502,343 @@
     </row>
     <row r="14" spans="1:26" ht="18">
       <c r="A14" s="1"/>
-      <c r="B14" s="141"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="54"/>
-      <c r="M14" s="55"/>
-      <c r="N14" s="56"/>
-      <c r="O14" s="55"/>
-      <c r="P14" s="57"/>
-      <c r="Q14" s="57"/>
-      <c r="R14" s="57"/>
-      <c r="S14" s="57"/>
-      <c r="T14" s="57"/>
-      <c r="U14" s="57"/>
-      <c r="V14" s="45"/>
-      <c r="W14" s="55"/>
-      <c r="X14" s="55"/>
-      <c r="Y14" s="54"/>
-      <c r="Z14" s="58"/>
+      <c r="B14" s="140"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="156"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="153"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="53"/>
+      <c r="M14" s="54"/>
+      <c r="N14" s="55"/>
+      <c r="O14" s="54"/>
+      <c r="P14" s="56"/>
+      <c r="Q14" s="56"/>
+      <c r="R14" s="56"/>
+      <c r="S14" s="56"/>
+      <c r="T14" s="56"/>
+      <c r="U14" s="56"/>
+      <c r="V14" s="44"/>
+      <c r="W14" s="54"/>
+      <c r="X14" s="54"/>
+      <c r="Y14" s="53"/>
+      <c r="Z14" s="57"/>
     </row>
     <row r="15" spans="1:26" ht="15">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="50"/>
-      <c r="L15" s="50"/>
-      <c r="M15" s="50"/>
-      <c r="N15" s="50"/>
-      <c r="O15" s="50"/>
-      <c r="P15" s="50"/>
-      <c r="Q15" s="50"/>
-      <c r="R15" s="50"/>
-      <c r="S15" s="50"/>
-      <c r="T15" s="50"/>
-      <c r="U15" s="50"/>
-      <c r="V15" s="50"/>
-      <c r="W15" s="50"/>
-      <c r="X15" s="50"/>
-      <c r="Y15" s="50"/>
-      <c r="Z15" s="59"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="49"/>
+      <c r="M15" s="49"/>
+      <c r="N15" s="49"/>
+      <c r="O15" s="49"/>
+      <c r="P15" s="49"/>
+      <c r="Q15" s="49"/>
+      <c r="R15" s="49"/>
+      <c r="S15" s="49"/>
+      <c r="T15" s="49"/>
+      <c r="U15" s="49"/>
+      <c r="V15" s="49"/>
+      <c r="W15" s="49"/>
+      <c r="X15" s="49"/>
+      <c r="Y15" s="49"/>
+      <c r="Z15" s="58"/>
     </row>
     <row r="16" spans="1:26" ht="15">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="50"/>
-      <c r="K16" s="50"/>
-      <c r="L16" s="50"/>
-      <c r="M16" s="50"/>
-      <c r="N16" s="50"/>
-      <c r="O16" s="50"/>
-      <c r="P16" s="50"/>
-      <c r="Q16" s="50"/>
-      <c r="R16" s="50"/>
-      <c r="S16" s="50"/>
-      <c r="T16" s="50"/>
-      <c r="U16" s="50"/>
-      <c r="V16" s="50"/>
-      <c r="W16" s="50"/>
-      <c r="X16" s="50"/>
-      <c r="Y16" s="50"/>
-      <c r="Z16" s="59"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="49"/>
+      <c r="L16" s="49"/>
+      <c r="M16" s="49"/>
+      <c r="N16" s="49"/>
+      <c r="O16" s="49"/>
+      <c r="P16" s="49"/>
+      <c r="Q16" s="49"/>
+      <c r="R16" s="49"/>
+      <c r="S16" s="49"/>
+      <c r="T16" s="49"/>
+      <c r="U16" s="49"/>
+      <c r="V16" s="49"/>
+      <c r="W16" s="49"/>
+      <c r="X16" s="49"/>
+      <c r="Y16" s="49"/>
+      <c r="Z16" s="58"/>
     </row>
     <row r="17" spans="1:26" ht="15">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="50"/>
-      <c r="K17" s="50"/>
-      <c r="L17" s="50"/>
-      <c r="M17" s="50"/>
-      <c r="N17" s="50"/>
-      <c r="O17" s="50"/>
-      <c r="P17" s="50"/>
-      <c r="Q17" s="50"/>
-      <c r="R17" s="50"/>
-      <c r="S17" s="50"/>
-      <c r="T17" s="50"/>
-      <c r="U17" s="50"/>
-      <c r="V17" s="50"/>
-      <c r="W17" s="50"/>
-      <c r="X17" s="50"/>
-      <c r="Y17" s="50"/>
-      <c r="Z17" s="59"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="49"/>
+      <c r="N17" s="49"/>
+      <c r="O17" s="49"/>
+      <c r="P17" s="49"/>
+      <c r="Q17" s="49"/>
+      <c r="R17" s="49"/>
+      <c r="S17" s="49"/>
+      <c r="T17" s="49"/>
+      <c r="U17" s="49"/>
+      <c r="V17" s="49"/>
+      <c r="W17" s="49"/>
+      <c r="X17" s="49"/>
+      <c r="Y17" s="49"/>
+      <c r="Z17" s="58"/>
     </row>
     <row r="18" spans="1:26" ht="15">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="50"/>
-      <c r="K18" s="50"/>
-      <c r="L18" s="50"/>
-      <c r="M18" s="50"/>
-      <c r="N18" s="50"/>
-      <c r="O18" s="50"/>
-      <c r="P18" s="50"/>
-      <c r="Q18" s="50"/>
-      <c r="R18" s="50"/>
-      <c r="S18" s="50"/>
-      <c r="T18" s="50"/>
-      <c r="U18" s="50"/>
-      <c r="V18" s="50"/>
-      <c r="W18" s="50"/>
-      <c r="X18" s="50"/>
-      <c r="Y18" s="50"/>
-      <c r="Z18" s="59"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="49"/>
+      <c r="M18" s="49"/>
+      <c r="N18" s="49"/>
+      <c r="O18" s="49"/>
+      <c r="P18" s="49"/>
+      <c r="Q18" s="49"/>
+      <c r="R18" s="49"/>
+      <c r="S18" s="49"/>
+      <c r="T18" s="49"/>
+      <c r="U18" s="49"/>
+      <c r="V18" s="49"/>
+      <c r="W18" s="49"/>
+      <c r="X18" s="49"/>
+      <c r="Y18" s="49"/>
+      <c r="Z18" s="58"/>
     </row>
     <row r="19" spans="1:26" ht="15">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
-      <c r="K19" s="50"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="50"/>
-      <c r="N19" s="50"/>
-      <c r="O19" s="50"/>
-      <c r="P19" s="50"/>
-      <c r="Q19" s="50"/>
-      <c r="R19" s="50"/>
-      <c r="S19" s="50"/>
-      <c r="T19" s="50"/>
-      <c r="U19" s="50"/>
-      <c r="V19" s="50"/>
-      <c r="W19" s="50"/>
-      <c r="X19" s="50"/>
-      <c r="Y19" s="50"/>
-      <c r="Z19" s="59"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="49"/>
+      <c r="L19" s="49"/>
+      <c r="M19" s="49"/>
+      <c r="N19" s="49"/>
+      <c r="O19" s="49"/>
+      <c r="P19" s="49"/>
+      <c r="Q19" s="49"/>
+      <c r="R19" s="49"/>
+      <c r="S19" s="49"/>
+      <c r="T19" s="49"/>
+      <c r="U19" s="49"/>
+      <c r="V19" s="49"/>
+      <c r="W19" s="49"/>
+      <c r="X19" s="49"/>
+      <c r="Y19" s="49"/>
+      <c r="Z19" s="58"/>
     </row>
     <row r="20" spans="1:26" ht="15">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="142" t="s">
+      <c r="C20" s="141" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="138"/>
-      <c r="E20" s="138"/>
-      <c r="F20" s="138"/>
-      <c r="G20" s="138"/>
-      <c r="H20" s="138"/>
-      <c r="I20" s="138"/>
-      <c r="J20" s="138"/>
-      <c r="K20" s="138"/>
-      <c r="L20" s="138"/>
-      <c r="M20" s="60"/>
-      <c r="N20" s="142" t="s">
+      <c r="D20" s="137"/>
+      <c r="E20" s="137"/>
+      <c r="F20" s="137"/>
+      <c r="G20" s="137"/>
+      <c r="H20" s="137"/>
+      <c r="I20" s="137"/>
+      <c r="J20" s="137"/>
+      <c r="K20" s="137"/>
+      <c r="L20" s="137"/>
+      <c r="M20" s="59"/>
+      <c r="N20" s="141" t="s">
         <v>44</v>
       </c>
-      <c r="O20" s="138"/>
-      <c r="P20" s="138"/>
-      <c r="Q20" s="138"/>
-      <c r="R20" s="138"/>
-      <c r="S20" s="138"/>
-      <c r="T20" s="138"/>
-      <c r="U20" s="138"/>
-      <c r="V20" s="138"/>
-      <c r="W20" s="138"/>
-      <c r="X20" s="50"/>
-      <c r="Y20" s="50"/>
-      <c r="Z20" s="59"/>
+      <c r="O20" s="137"/>
+      <c r="P20" s="137"/>
+      <c r="Q20" s="137"/>
+      <c r="R20" s="137"/>
+      <c r="S20" s="137"/>
+      <c r="T20" s="137"/>
+      <c r="U20" s="137"/>
+      <c r="V20" s="137"/>
+      <c r="W20" s="137"/>
+      <c r="X20" s="49"/>
+      <c r="Y20" s="49"/>
+      <c r="Z20" s="58"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="61">
+      <c r="C21" s="60">
         <v>10</v>
       </c>
-      <c r="D21" s="61">
+      <c r="D21" s="60">
         <v>20</v>
       </c>
-      <c r="E21" s="61">
+      <c r="E21" s="60">
         <v>30</v>
       </c>
-      <c r="F21" s="61">
+      <c r="F21" s="60">
         <v>40</v>
       </c>
-      <c r="G21" s="61">
+      <c r="G21" s="60">
         <v>50</v>
       </c>
-      <c r="H21" s="61">
+      <c r="H21" s="60">
         <v>60</v>
       </c>
-      <c r="I21" s="61">
+      <c r="I21" s="60">
         <v>70</v>
       </c>
-      <c r="J21" s="61">
+      <c r="J21" s="60">
         <v>80</v>
       </c>
-      <c r="K21" s="61">
+      <c r="K21" s="60">
         <v>90</v>
       </c>
-      <c r="L21" s="61">
+      <c r="L21" s="60">
         <v>100</v>
       </c>
-      <c r="M21" s="61">
+      <c r="M21" s="60">
         <v>110</v>
       </c>
-      <c r="N21" s="61">
+      <c r="N21" s="60">
         <v>120</v>
       </c>
-      <c r="O21" s="61">
+      <c r="O21" s="60">
         <v>130</v>
       </c>
-      <c r="P21" s="61">
+      <c r="P21" s="60">
         <v>140</v>
       </c>
-      <c r="Q21" s="61">
+      <c r="Q21" s="60">
         <v>150</v>
       </c>
-      <c r="R21" s="61">
+      <c r="R21" s="60">
         <v>160</v>
       </c>
-      <c r="S21" s="61">
+      <c r="S21" s="60">
         <v>170</v>
       </c>
-      <c r="T21" s="61">
+      <c r="T21" s="60">
         <v>180</v>
       </c>
-      <c r="U21" s="61">
+      <c r="U21" s="60">
         <v>190</v>
       </c>
-      <c r="V21" s="61">
+      <c r="V21" s="60">
         <v>200</v>
       </c>
-      <c r="W21" s="61">
+      <c r="W21" s="60">
         <v>210</v>
       </c>
-      <c r="X21" s="61">
+      <c r="X21" s="60">
         <v>220</v>
       </c>
-      <c r="Y21" s="50"/>
-      <c r="Z21" s="59"/>
+      <c r="Y21" s="49"/>
+      <c r="Z21" s="58"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A22" s="139" t="s">
+      <c r="A22" s="138" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="139" t="s">
+      <c r="B22" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="62" t="s">
+      <c r="C22" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="63" t="s">
+      <c r="D22" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="64" t="s">
+      <c r="E22" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="64" t="s">
+      <c r="F22" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="64" t="s">
+      <c r="G22" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="H22" s="64" t="s">
+      <c r="H22" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="62" t="s">
+      <c r="I22" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="J22" s="65" t="s">
+      <c r="J22" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="K22" s="63"/>
-      <c r="L22" s="66"/>
-      <c r="M22" s="63"/>
-      <c r="N22" s="62" t="s">
+      <c r="K22" s="62"/>
+      <c r="L22" s="65"/>
+      <c r="M22" s="62"/>
+      <c r="N22" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="O22" s="63" t="s">
+      <c r="O22" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="P22" s="64" t="s">
+      <c r="P22" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="Q22" s="64" t="s">
+      <c r="Q22" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="R22" s="64" t="s">
+      <c r="R22" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="S22" s="64" t="s">
+      <c r="S22" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="T22" s="64" t="s">
+      <c r="T22" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="U22" s="67" t="s">
+      <c r="U22" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="V22" s="68"/>
-      <c r="W22" s="69"/>
-      <c r="X22" s="69"/>
-      <c r="Y22" s="70"/>
-      <c r="Z22" s="71"/>
+      <c r="V22" s="67"/>
+      <c r="W22" s="68"/>
+      <c r="X22" s="68"/>
+      <c r="Y22" s="69"/>
+      <c r="Z22" s="70"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A23" s="140"/>
-      <c r="B23" s="140"/>
+      <c r="A23" s="139"/>
+      <c r="B23" s="139"/>
       <c r="C23" s="29" t="s">
         <v>28</v>
       </c>
@@ -2855,10 +2891,10 @@
       <c r="T23" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="U23" s="46" t="s">
+      <c r="U23" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="V23" s="72"/>
+      <c r="V23" s="71"/>
       <c r="W23" s="28" t="s">
         <v>32</v>
       </c>
@@ -2873,8 +2909,8 @@
       </c>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A24" s="140"/>
-      <c r="B24" s="140"/>
+      <c r="A24" s="139"/>
+      <c r="B24" s="139"/>
       <c r="C24" s="29"/>
       <c r="D24" s="28"/>
       <c r="E24" s="30"/>
@@ -2893,16 +2929,16 @@
       <c r="R24" s="30"/>
       <c r="S24" s="30"/>
       <c r="T24" s="30"/>
-      <c r="U24" s="46"/>
-      <c r="V24" s="72"/>
+      <c r="U24" s="45"/>
+      <c r="V24" s="71"/>
       <c r="W24" s="33"/>
       <c r="X24" s="33"/>
       <c r="Y24" s="34"/>
       <c r="Z24" s="35"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A25" s="140"/>
-      <c r="B25" s="140"/>
+      <c r="A25" s="139"/>
+      <c r="B25" s="139"/>
       <c r="C25" s="29"/>
       <c r="D25" s="28"/>
       <c r="E25" s="30"/>
@@ -2921,36 +2957,36 @@
       <c r="R25" s="30"/>
       <c r="S25" s="30"/>
       <c r="T25" s="30"/>
-      <c r="U25" s="46"/>
-      <c r="V25" s="72"/>
+      <c r="U25" s="45"/>
+      <c r="V25" s="71"/>
       <c r="W25" s="33"/>
       <c r="X25" s="33"/>
       <c r="Y25" s="34"/>
       <c r="Z25" s="35"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A26" s="141"/>
-      <c r="B26" s="140"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="44"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="73"/>
+      <c r="A26" s="140"/>
+      <c r="B26" s="139"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="72"/>
       <c r="K26" s="28"/>
-      <c r="L26" s="41"/>
+      <c r="L26" s="40"/>
       <c r="M26" s="28"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="43"/>
-      <c r="P26" s="44"/>
-      <c r="Q26" s="44"/>
-      <c r="R26" s="44"/>
-      <c r="S26" s="44"/>
-      <c r="T26" s="44"/>
-      <c r="U26" s="57"/>
-      <c r="V26" s="74"/>
+      <c r="N26" s="41"/>
+      <c r="O26" s="42"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="43"/>
+      <c r="S26" s="43"/>
+      <c r="T26" s="43"/>
+      <c r="U26" s="56"/>
+      <c r="V26" s="73"/>
       <c r="W26" s="33"/>
       <c r="X26" s="33"/>
       <c r="Y26" s="34"/>
@@ -2958,7 +2994,7 @@
     </row>
     <row r="27" spans="1:26" ht="15">
       <c r="A27" s="1"/>
-      <c r="B27" s="140"/>
+      <c r="B27" s="139"/>
       <c r="C27" s="29" t="s">
         <v>6</v>
       </c>
@@ -3007,10 +3043,10 @@
       <c r="T27" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="U27" s="46" t="s">
+      <c r="U27" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="V27" s="72"/>
+      <c r="V27" s="71"/>
       <c r="W27" s="33"/>
       <c r="X27" s="33"/>
       <c r="Y27" s="34"/>
@@ -3018,7 +3054,7 @@
     </row>
     <row r="28" spans="1:26" ht="23">
       <c r="A28" s="1"/>
-      <c r="B28" s="140"/>
+      <c r="B28" s="139"/>
       <c r="C28" s="29" t="s">
         <v>19</v>
       </c>
@@ -3070,7 +3106,7 @@
       <c r="U28" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="V28" s="75"/>
+      <c r="V28" s="74"/>
       <c r="W28" s="28"/>
       <c r="X28" s="28"/>
       <c r="Y28" s="27"/>
@@ -3078,87 +3114,87 @@
     </row>
     <row r="29" spans="1:26" ht="15">
       <c r="A29" s="1"/>
-      <c r="B29" s="140"/>
+      <c r="B29" s="139"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="76"/>
-      <c r="E29" s="77"/>
-      <c r="F29" s="77"/>
-      <c r="G29" s="77"/>
-      <c r="H29" s="77"/>
+      <c r="D29" s="75"/>
+      <c r="E29" s="76"/>
+      <c r="F29" s="76"/>
+      <c r="G29" s="76"/>
+      <c r="H29" s="76"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="78"/>
-      <c r="K29" s="76"/>
-      <c r="L29" s="79"/>
-      <c r="M29" s="76"/>
-      <c r="N29" s="80"/>
-      <c r="O29" s="81"/>
-      <c r="P29" s="82"/>
-      <c r="Q29" s="82"/>
-      <c r="R29" s="82"/>
-      <c r="S29" s="82"/>
-      <c r="T29" s="82"/>
-      <c r="U29" s="82"/>
-      <c r="V29" s="83"/>
-      <c r="W29" s="81"/>
-      <c r="X29" s="84"/>
-      <c r="Y29" s="85"/>
-      <c r="Z29" s="86"/>
+      <c r="J29" s="77"/>
+      <c r="K29" s="75"/>
+      <c r="L29" s="78"/>
+      <c r="M29" s="75"/>
+      <c r="N29" s="79"/>
+      <c r="O29" s="80"/>
+      <c r="P29" s="81"/>
+      <c r="Q29" s="81"/>
+      <c r="R29" s="81"/>
+      <c r="S29" s="81"/>
+      <c r="T29" s="81"/>
+      <c r="U29" s="81"/>
+      <c r="V29" s="82"/>
+      <c r="W29" s="80"/>
+      <c r="X29" s="83"/>
+      <c r="Y29" s="84"/>
+      <c r="Z29" s="85"/>
     </row>
     <row r="30" spans="1:26" ht="15">
       <c r="A30" s="1"/>
-      <c r="B30" s="140"/>
+      <c r="B30" s="139"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="76"/>
-      <c r="E30" s="77"/>
-      <c r="F30" s="77"/>
-      <c r="G30" s="77"/>
-      <c r="H30" s="77"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="76"/>
+      <c r="F30" s="76"/>
+      <c r="G30" s="76"/>
+      <c r="H30" s="76"/>
       <c r="I30" s="2"/>
-      <c r="J30" s="78"/>
-      <c r="K30" s="76"/>
-      <c r="L30" s="79"/>
-      <c r="M30" s="76"/>
-      <c r="N30" s="80"/>
-      <c r="O30" s="81"/>
-      <c r="P30" s="82"/>
-      <c r="Q30" s="82"/>
-      <c r="R30" s="82"/>
-      <c r="S30" s="82"/>
-      <c r="T30" s="82"/>
-      <c r="U30" s="82"/>
-      <c r="V30" s="83"/>
-      <c r="W30" s="81"/>
-      <c r="X30" s="84"/>
-      <c r="Y30" s="85"/>
-      <c r="Z30" s="86"/>
+      <c r="J30" s="77"/>
+      <c r="K30" s="75"/>
+      <c r="L30" s="78"/>
+      <c r="M30" s="75"/>
+      <c r="N30" s="79"/>
+      <c r="O30" s="80"/>
+      <c r="P30" s="81"/>
+      <c r="Q30" s="81"/>
+      <c r="R30" s="81"/>
+      <c r="S30" s="81"/>
+      <c r="T30" s="81"/>
+      <c r="U30" s="81"/>
+      <c r="V30" s="82"/>
+      <c r="W30" s="80"/>
+      <c r="X30" s="83"/>
+      <c r="Y30" s="84"/>
+      <c r="Z30" s="85"/>
     </row>
     <row r="31" spans="1:26" ht="15">
       <c r="A31" s="1"/>
-      <c r="B31" s="141"/>
-      <c r="C31" s="87"/>
-      <c r="D31" s="88"/>
-      <c r="E31" s="89"/>
-      <c r="F31" s="89"/>
-      <c r="G31" s="89"/>
-      <c r="H31" s="89"/>
-      <c r="I31" s="87"/>
-      <c r="J31" s="90"/>
-      <c r="K31" s="88"/>
-      <c r="L31" s="91"/>
-      <c r="M31" s="88"/>
-      <c r="N31" s="92"/>
-      <c r="O31" s="93"/>
-      <c r="P31" s="94"/>
-      <c r="Q31" s="94"/>
-      <c r="R31" s="94"/>
-      <c r="S31" s="94"/>
-      <c r="T31" s="94"/>
-      <c r="U31" s="94"/>
-      <c r="V31" s="95"/>
-      <c r="W31" s="93"/>
-      <c r="X31" s="96"/>
-      <c r="Y31" s="97"/>
-      <c r="Z31" s="98"/>
+      <c r="B31" s="140"/>
+      <c r="C31" s="86"/>
+      <c r="D31" s="87"/>
+      <c r="E31" s="88"/>
+      <c r="F31" s="88"/>
+      <c r="G31" s="88"/>
+      <c r="H31" s="88"/>
+      <c r="I31" s="86"/>
+      <c r="J31" s="89"/>
+      <c r="K31" s="87"/>
+      <c r="L31" s="90"/>
+      <c r="M31" s="87"/>
+      <c r="N31" s="91"/>
+      <c r="O31" s="92"/>
+      <c r="P31" s="93"/>
+      <c r="Q31" s="93"/>
+      <c r="R31" s="93"/>
+      <c r="S31" s="93"/>
+      <c r="T31" s="93"/>
+      <c r="U31" s="93"/>
+      <c r="V31" s="94"/>
+      <c r="W31" s="92"/>
+      <c r="X31" s="95"/>
+      <c r="Y31" s="96"/>
+      <c r="Z31" s="97"/>
     </row>
     <row r="32" spans="1:26" ht="15">
       <c r="A32" s="1"/>
@@ -3191,19 +3227,19 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
-      <c r="I33" s="99" t="s">
+      <c r="I33" s="98" t="s">
         <v>49</v>
       </c>
-      <c r="J33" s="99" t="s">
+      <c r="J33" s="98" t="s">
         <v>50</v>
       </c>
-      <c r="K33" s="99" t="s">
+      <c r="K33" s="98" t="s">
         <v>51</v>
       </c>
-      <c r="L33" s="99" t="s">
+      <c r="L33" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="M33" s="99" t="s">
+      <c r="M33" s="98" t="s">
         <v>53</v>
       </c>
       <c r="N33" s="1"/>
@@ -3228,19 +3264,19 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
-      <c r="I34" s="99" t="s">
+      <c r="I34" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="J34" s="100" t="s">
+      <c r="J34" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="K34" s="100" t="s">
+      <c r="K34" s="99" t="s">
         <v>55</v>
       </c>
-      <c r="L34" s="100" t="s">
+      <c r="L34" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="M34" s="99" t="s">
+      <c r="M34" s="98" t="s">
         <v>57</v>
       </c>
       <c r="N34" s="1"/>
@@ -3265,19 +3301,19 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
-      <c r="I35" s="99" t="s">
+      <c r="I35" s="98" t="s">
         <v>58</v>
       </c>
-      <c r="J35" s="100" t="s">
+      <c r="J35" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="K35" s="100" t="s">
+      <c r="K35" s="99" t="s">
         <v>59</v>
       </c>
-      <c r="L35" s="100" t="s">
+      <c r="L35" s="99" t="s">
         <v>60</v>
       </c>
-      <c r="M35" s="99" t="s">
+      <c r="M35" s="98" t="s">
         <v>61</v>
       </c>
       <c r="N35" s="1"/>
@@ -3302,19 +3338,19 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
-      <c r="I36" s="99" t="s">
+      <c r="I36" s="98" t="s">
         <v>62</v>
       </c>
-      <c r="J36" s="100" t="s">
+      <c r="J36" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="K36" s="100" t="s">
+      <c r="K36" s="99" t="s">
         <v>63</v>
       </c>
-      <c r="L36" s="100" t="s">
+      <c r="L36" s="99" t="s">
         <v>64</v>
       </c>
-      <c r="M36" s="99" t="s">
+      <c r="M36" s="98" t="s">
         <v>65</v>
       </c>
       <c r="N36" s="1"/>
@@ -3339,19 +3375,19 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
-      <c r="I37" s="99" t="s">
+      <c r="I37" s="98" t="s">
         <v>66</v>
       </c>
-      <c r="J37" s="100" t="s">
+      <c r="J37" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="K37" s="100" t="s">
+      <c r="K37" s="99" t="s">
         <v>67</v>
       </c>
-      <c r="L37" s="100" t="s">
+      <c r="L37" s="99" t="s">
         <v>68</v>
       </c>
-      <c r="M37" s="99" t="s">
+      <c r="M37" s="98" t="s">
         <v>69</v>
       </c>
       <c r="N37" s="1"/>
@@ -3376,19 +3412,19 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
-      <c r="I38" s="99" t="s">
+      <c r="I38" s="98" t="s">
         <v>70</v>
       </c>
-      <c r="J38" s="100" t="s">
+      <c r="J38" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="K38" s="100" t="s">
+      <c r="K38" s="99" t="s">
         <v>71</v>
       </c>
-      <c r="L38" s="100" t="s">
+      <c r="L38" s="99" t="s">
         <v>72</v>
       </c>
-      <c r="M38" s="99" t="s">
+      <c r="M38" s="98" t="s">
         <v>73</v>
       </c>
       <c r="N38" s="1"/>
@@ -3413,19 +3449,19 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
-      <c r="I39" s="99" t="s">
+      <c r="I39" s="98" t="s">
         <v>74</v>
       </c>
-      <c r="J39" s="100" t="s">
+      <c r="J39" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="K39" s="100" t="s">
+      <c r="K39" s="99" t="s">
         <v>75</v>
       </c>
-      <c r="L39" s="100" t="s">
+      <c r="L39" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="M39" s="99" t="s">
+      <c r="M39" s="98" t="s">
         <v>77</v>
       </c>
       <c r="N39" s="1"/>
@@ -3450,19 +3486,19 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
-      <c r="I40" s="99" t="s">
+      <c r="I40" s="98" t="s">
         <v>78</v>
       </c>
-      <c r="J40" s="100" t="s">
+      <c r="J40" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="K40" s="100" t="s">
+      <c r="K40" s="99" t="s">
         <v>79</v>
       </c>
-      <c r="L40" s="100" t="s">
+      <c r="L40" s="99" t="s">
         <v>80</v>
       </c>
-      <c r="M40" s="99" t="s">
+      <c r="M40" s="98" t="s">
         <v>81</v>
       </c>
       <c r="N40" s="1"/>
@@ -3487,19 +3523,19 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
-      <c r="I41" s="99" t="s">
+      <c r="I41" s="98" t="s">
         <v>82</v>
       </c>
-      <c r="J41" s="100" t="s">
+      <c r="J41" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="K41" s="100" t="s">
+      <c r="K41" s="99" t="s">
         <v>47</v>
       </c>
-      <c r="L41" s="100" t="s">
+      <c r="L41" s="99" t="s">
         <v>83</v>
       </c>
-      <c r="M41" s="99" t="s">
+      <c r="M41" s="98" t="s">
         <v>84</v>
       </c>
       <c r="N41" s="1"/>
@@ -3524,19 +3560,19 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
-      <c r="I42" s="99" t="s">
+      <c r="I42" s="98" t="s">
         <v>85</v>
       </c>
-      <c r="J42" s="100" t="s">
+      <c r="J42" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="K42" s="100" t="s">
+      <c r="K42" s="99" t="s">
         <v>86</v>
       </c>
-      <c r="L42" s="100" t="s">
+      <c r="L42" s="99" t="s">
         <v>87</v>
       </c>
-      <c r="M42" s="99" t="s">
+      <c r="M42" s="98" t="s">
         <v>88</v>
       </c>
       <c r="N42" s="1"/>
@@ -3561,19 +3597,19 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
-      <c r="I43" s="99" t="s">
+      <c r="I43" s="98" t="s">
         <v>89</v>
       </c>
-      <c r="J43" s="100" t="s">
+      <c r="J43" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="K43" s="100" t="s">
+      <c r="K43" s="99" t="s">
         <v>90</v>
       </c>
-      <c r="L43" s="100" t="s">
+      <c r="L43" s="99" t="s">
         <v>91</v>
       </c>
-      <c r="M43" s="99" t="s">
+      <c r="M43" s="98" t="s">
         <v>92</v>
       </c>
       <c r="N43" s="1"/>
@@ -3598,19 +3634,19 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
-      <c r="I44" s="99" t="s">
+      <c r="I44" s="98" t="s">
         <v>93</v>
       </c>
-      <c r="J44" s="100" t="s">
+      <c r="J44" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="K44" s="100" t="s">
+      <c r="K44" s="99" t="s">
         <v>94</v>
       </c>
-      <c r="L44" s="100" t="s">
+      <c r="L44" s="99" t="s">
         <v>95</v>
       </c>
-      <c r="M44" s="99" t="s">
+      <c r="M44" s="98" t="s">
         <v>96</v>
       </c>
       <c r="N44" s="1"/>
@@ -3635,19 +3671,19 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
-      <c r="I45" s="99" t="s">
+      <c r="I45" s="98" t="s">
         <v>97</v>
       </c>
-      <c r="J45" s="100" t="s">
+      <c r="J45" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="K45" s="100" t="s">
+      <c r="K45" s="99" t="s">
         <v>98</v>
       </c>
-      <c r="L45" s="100" t="s">
+      <c r="L45" s="99" t="s">
         <v>99</v>
       </c>
-      <c r="M45" s="99" t="s">
+      <c r="M45" s="98" t="s">
         <v>100</v>
       </c>
       <c r="N45" s="1"/>
@@ -3670,19 +3706,19 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-      <c r="I46" s="99" t="s">
+      <c r="I46" s="98" t="s">
         <v>101</v>
       </c>
-      <c r="J46" s="100" t="s">
+      <c r="J46" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="K46" s="100" t="s">
+      <c r="K46" s="99" t="s">
         <v>102</v>
       </c>
-      <c r="L46" s="100" t="s">
+      <c r="L46" s="99" t="s">
         <v>103</v>
       </c>
-      <c r="M46" s="99" t="s">
+      <c r="M46" s="98" t="s">
         <v>104</v>
       </c>
       <c r="N46" s="1"/>
@@ -3705,17 +3741,17 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
-      <c r="I47" s="99" t="s">
+      <c r="I47" s="157" t="s">
         <v>105</v>
       </c>
-      <c r="J47" s="100" t="s">
+      <c r="J47" s="158" t="s">
         <v>12</v>
       </c>
-      <c r="K47" s="99"/>
-      <c r="L47" s="100" t="s">
+      <c r="K47" s="157"/>
+      <c r="L47" s="158" t="s">
         <v>18</v>
       </c>
-      <c r="M47" s="99" t="s">
+      <c r="M47" s="157" t="s">
         <v>106</v>
       </c>
       <c r="N47" s="1"/>
@@ -3738,17 +3774,17 @@
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
-      <c r="I48" s="99" t="s">
+      <c r="I48" s="157" t="s">
         <v>107</v>
       </c>
-      <c r="J48" s="100" t="s">
+      <c r="J48" s="158" t="s">
         <v>5</v>
       </c>
-      <c r="K48" s="99"/>
-      <c r="L48" s="100" t="s">
+      <c r="K48" s="157"/>
+      <c r="L48" s="158" t="s">
         <v>18</v>
       </c>
-      <c r="M48" s="99" t="s">
+      <c r="M48" s="157" t="s">
         <v>106</v>
       </c>
       <c r="N48" s="1"/>
@@ -3771,17 +3807,17 @@
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
-      <c r="I49" s="99" t="s">
+      <c r="I49" s="157" t="s">
         <v>108</v>
       </c>
-      <c r="J49" s="100" t="s">
+      <c r="J49" s="158" t="s">
         <v>37</v>
       </c>
-      <c r="K49" s="99"/>
-      <c r="L49" s="100" t="s">
+      <c r="K49" s="157"/>
+      <c r="L49" s="158" t="s">
         <v>18</v>
       </c>
-      <c r="M49" s="99" t="s">
+      <c r="M49" s="157" t="s">
         <v>106</v>
       </c>
       <c r="N49" s="1"/>
@@ -3829,9 +3865,9 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
-      <c r="I51" s="134"/>
-      <c r="J51" s="135"/>
-      <c r="K51" s="135"/>
+      <c r="I51" s="133"/>
+      <c r="J51" s="134"/>
+      <c r="K51" s="134"/>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
@@ -3879,9 +3915,9 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
-      <c r="I53" s="134"/>
-      <c r="J53" s="135"/>
-      <c r="K53" s="135"/>
+      <c r="I53" s="133"/>
+      <c r="J53" s="134"/>
+      <c r="K53" s="134"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
@@ -3904,9 +3940,9 @@
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
-      <c r="I54" s="134"/>
-      <c r="J54" s="135"/>
-      <c r="K54" s="135"/>
+      <c r="I54" s="133"/>
+      <c r="J54" s="134"/>
+      <c r="K54" s="134"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
@@ -3929,9 +3965,9 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
-      <c r="I55" s="134"/>
-      <c r="J55" s="135"/>
-      <c r="K55" s="135"/>
+      <c r="I55" s="133"/>
+      <c r="J55" s="134"/>
+      <c r="K55" s="134"/>
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
@@ -4073,13 +4109,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="100" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="101" t="s">
+      <c r="B1" s="100" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="101" t="s">
+      <c r="C1" s="100" t="s">
         <v>111</v>
       </c>
     </row>
@@ -4087,10 +4123,10 @@
       <c r="A2" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="102">
+      <c r="B2" s="101">
         <v>44643</v>
       </c>
-      <c r="C2" s="103" t="s">
+      <c r="C2" s="102" t="s">
         <v>113</v>
       </c>
     </row>
@@ -4145,1106 +4181,1106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="15.75" customHeight="1">
-      <c r="A1" s="103"/>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
-      <c r="G1" s="104"/>
-      <c r="H1" s="104"/>
-      <c r="I1" s="104"/>
-      <c r="J1" s="104"/>
-      <c r="K1" s="104"/>
-      <c r="L1" s="104"/>
-      <c r="M1" s="143" t="s">
+      <c r="A1" s="102"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="142" t="s">
         <v>114</v>
       </c>
-      <c r="N1" s="135"/>
-      <c r="O1" s="135"/>
-      <c r="P1" s="135"/>
-      <c r="Q1" s="135"/>
-      <c r="R1" s="135"/>
-      <c r="S1" s="135"/>
-      <c r="T1" s="144" t="s">
+      <c r="N1" s="134"/>
+      <c r="O1" s="134"/>
+      <c r="P1" s="134"/>
+      <c r="Q1" s="134"/>
+      <c r="R1" s="134"/>
+      <c r="S1" s="134"/>
+      <c r="T1" s="143" t="s">
         <v>115</v>
       </c>
-      <c r="U1" s="135"/>
-      <c r="V1" s="135"/>
-      <c r="W1" s="135"/>
-      <c r="X1" s="135"/>
-      <c r="Y1" s="135"/>
-      <c r="Z1" s="135"/>
-      <c r="AA1" s="135"/>
-      <c r="AB1" s="135"/>
-      <c r="AC1" s="145" t="s">
+      <c r="U1" s="134"/>
+      <c r="V1" s="134"/>
+      <c r="W1" s="134"/>
+      <c r="X1" s="134"/>
+      <c r="Y1" s="134"/>
+      <c r="Z1" s="134"/>
+      <c r="AA1" s="134"/>
+      <c r="AB1" s="134"/>
+      <c r="AC1" s="144" t="s">
         <v>116</v>
       </c>
-      <c r="AD1" s="135"/>
-      <c r="AE1" s="135"/>
-      <c r="AF1" s="135"/>
+      <c r="AD1" s="134"/>
+      <c r="AE1" s="134"/>
+      <c r="AF1" s="134"/>
     </row>
     <row r="2" spans="1:35" ht="15.75" customHeight="1">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="102" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="102" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="103" t="s">
+      <c r="C2" s="102" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="105" t="s">
+      <c r="D2" s="104" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="105" t="s">
+      <c r="E2" s="104" t="s">
         <v>121</v>
       </c>
-      <c r="F2" s="105" t="s">
+      <c r="F2" s="104" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="105" t="s">
+      <c r="G2" s="104" t="s">
         <v>123</v>
       </c>
-      <c r="H2" s="105" t="s">
+      <c r="H2" s="104" t="s">
         <v>124</v>
       </c>
-      <c r="I2" s="105" t="s">
+      <c r="I2" s="104" t="s">
         <v>125</v>
       </c>
-      <c r="J2" s="105" t="s">
+      <c r="J2" s="104" t="s">
         <v>126</v>
       </c>
-      <c r="K2" s="105" t="s">
+      <c r="K2" s="104" t="s">
         <v>127</v>
       </c>
-      <c r="L2" s="105" t="s">
+      <c r="L2" s="104" t="s">
         <v>128</v>
       </c>
-      <c r="M2" s="105" t="s">
+      <c r="M2" s="104" t="s">
         <v>129</v>
       </c>
-      <c r="N2" s="105" t="s">
+      <c r="N2" s="104" t="s">
         <v>130</v>
       </c>
-      <c r="O2" s="105" t="s">
+      <c r="O2" s="104" t="s">
         <v>131</v>
       </c>
-      <c r="P2" s="105" t="s">
+      <c r="P2" s="104" t="s">
         <v>132</v>
       </c>
-      <c r="Q2" s="105" t="s">
+      <c r="Q2" s="104" t="s">
         <v>133</v>
       </c>
-      <c r="R2" s="105" t="s">
+      <c r="R2" s="104" t="s">
         <v>134</v>
       </c>
-      <c r="S2" s="105" t="s">
+      <c r="S2" s="104" t="s">
         <v>135</v>
       </c>
-      <c r="T2" s="106" t="s">
+      <c r="T2" s="105" t="s">
         <v>136</v>
       </c>
-      <c r="U2" s="106" t="s">
+      <c r="U2" s="105" t="s">
         <v>137</v>
       </c>
-      <c r="V2" s="106" t="s">
+      <c r="V2" s="105" t="s">
         <v>138</v>
       </c>
-      <c r="W2" s="106" t="s">
+      <c r="W2" s="105" t="s">
         <v>139</v>
       </c>
-      <c r="X2" s="106" t="s">
+      <c r="X2" s="105" t="s">
         <v>140</v>
       </c>
-      <c r="Y2" s="106" t="s">
+      <c r="Y2" s="105" t="s">
         <v>141</v>
       </c>
-      <c r="Z2" s="106" t="s">
+      <c r="Z2" s="105" t="s">
         <v>142</v>
       </c>
-      <c r="AA2" s="106" t="s">
+      <c r="AA2" s="105" t="s">
         <v>143</v>
       </c>
-      <c r="AB2" s="106" t="s">
+      <c r="AB2" s="105" t="s">
         <v>144</v>
       </c>
-      <c r="AC2" s="107" t="s">
+      <c r="AC2" s="106" t="s">
         <v>145</v>
       </c>
-      <c r="AD2" s="107" t="s">
+      <c r="AD2" s="106" t="s">
         <v>146</v>
       </c>
-      <c r="AE2" s="107" t="s">
+      <c r="AE2" s="106" t="s">
         <v>147</v>
       </c>
-      <c r="AF2" s="107" t="s">
+      <c r="AF2" s="106" t="s">
         <v>148</v>
       </c>
-      <c r="AG2" s="103" t="s">
+      <c r="AG2" s="102" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="15.75" customHeight="1">
-      <c r="A3" s="103" t="s">
+      <c r="A3" s="102" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="103" t="s">
+      <c r="B3" s="102" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="103">
+      <c r="D3" s="102">
         <v>15</v>
       </c>
-      <c r="E3" s="103">
+      <c r="E3" s="102">
         <v>93</v>
       </c>
-      <c r="F3" s="103">
+      <c r="F3" s="102">
         <v>99.45</v>
       </c>
-      <c r="G3" s="108">
+      <c r="G3" s="107">
         <f t="shared" ref="G3:G17" si="0">D3/(E3/100)/(F3/100)</f>
         <v>16.218232537018114</v>
       </c>
-      <c r="H3" s="109">
+      <c r="H3" s="108">
         <f t="shared" ref="H3:H17" si="1">G3*((10*25)/43560)</f>
         <v>9.3079846975540129E-2</v>
       </c>
-      <c r="I3" s="108">
+      <c r="I3" s="107">
         <f t="shared" ref="I3:I17" si="2">H3*454</f>
         <v>42.258250526895218</v>
       </c>
-      <c r="J3" s="103">
+      <c r="J3" s="102">
         <v>1.9</v>
       </c>
-      <c r="K3" s="108">
+      <c r="K3" s="107">
         <f t="shared" ref="K3:K13" si="3">G3*J3</f>
         <v>30.814641820334415</v>
       </c>
-      <c r="M3" s="103"/>
-      <c r="N3" s="103"/>
-      <c r="O3" s="103"/>
-      <c r="P3" s="103"/>
-      <c r="Q3" s="103"/>
-      <c r="R3" s="103"/>
-      <c r="S3" s="103"/>
-      <c r="T3" s="103"/>
-      <c r="U3" s="103"/>
-      <c r="V3" s="103"/>
-      <c r="W3" s="103"/>
-      <c r="X3" s="103"/>
-      <c r="Y3" s="103"/>
-      <c r="Z3" s="103"/>
-      <c r="AA3" s="103"/>
-      <c r="AB3" s="103"/>
-      <c r="AC3" s="103"/>
-      <c r="AD3" s="103"/>
-      <c r="AE3" s="110"/>
-      <c r="AF3" s="110"/>
+      <c r="M3" s="102"/>
+      <c r="N3" s="102"/>
+      <c r="O3" s="102"/>
+      <c r="P3" s="102"/>
+      <c r="Q3" s="102"/>
+      <c r="R3" s="102"/>
+      <c r="S3" s="102"/>
+      <c r="T3" s="102"/>
+      <c r="U3" s="102"/>
+      <c r="V3" s="102"/>
+      <c r="W3" s="102"/>
+      <c r="X3" s="102"/>
+      <c r="Y3" s="102"/>
+      <c r="Z3" s="102"/>
+      <c r="AA3" s="102"/>
+      <c r="AB3" s="102"/>
+      <c r="AC3" s="102"/>
+      <c r="AD3" s="102"/>
+      <c r="AE3" s="109"/>
+      <c r="AF3" s="109"/>
     </row>
     <row r="4" spans="1:35" ht="15.75" customHeight="1">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="102" t="s">
         <v>150</v>
       </c>
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="102" t="s">
         <v>151</v>
       </c>
-      <c r="C4" s="110"/>
-      <c r="D4" s="103">
+      <c r="C4" s="109"/>
+      <c r="D4" s="102">
         <v>10</v>
       </c>
-      <c r="E4" s="103">
+      <c r="E4" s="102">
         <v>94</v>
       </c>
-      <c r="F4" s="103">
+      <c r="F4" s="102">
         <v>99.94</v>
       </c>
-      <c r="G4" s="108">
+      <c r="G4" s="107">
         <f t="shared" si="0"/>
         <v>10.644684683150317</v>
       </c>
-      <c r="H4" s="109">
+      <c r="H4" s="108">
         <f t="shared" si="1"/>
         <v>6.1092083810550479E-2</v>
       </c>
-      <c r="I4" s="108">
+      <c r="I4" s="107">
         <f t="shared" si="2"/>
         <v>27.735806049989918</v>
       </c>
-      <c r="J4" s="103">
+      <c r="J4" s="102">
         <v>1.75</v>
       </c>
-      <c r="K4" s="108">
+      <c r="K4" s="107">
         <f t="shared" si="3"/>
         <v>18.628198195513054</v>
       </c>
-      <c r="L4" s="111" t="s">
+      <c r="L4" s="110" t="s">
         <v>152</v>
       </c>
-      <c r="M4" s="103" t="s">
+      <c r="M4" s="102" t="s">
         <v>153</v>
       </c>
-      <c r="N4" s="103">
+      <c r="N4" s="102">
         <v>170000</v>
       </c>
-      <c r="O4" s="103" t="s">
+      <c r="O4" s="102" t="s">
         <v>154</v>
       </c>
-      <c r="P4" s="103" t="s">
+      <c r="P4" s="102" t="s">
         <v>155</v>
       </c>
-      <c r="Q4" s="103" t="s">
+      <c r="Q4" s="102" t="s">
         <v>156</v>
       </c>
-      <c r="R4" s="103">
+      <c r="R4" s="102">
         <v>10</v>
       </c>
-      <c r="S4" s="103" t="s">
+      <c r="S4" s="102" t="s">
         <v>157</v>
       </c>
-      <c r="T4" s="103" t="s">
+      <c r="T4" s="102" t="s">
         <v>158</v>
       </c>
-      <c r="U4" s="103" t="s">
+      <c r="U4" s="102" t="s">
         <v>159</v>
       </c>
-      <c r="V4" s="103" t="s">
+      <c r="V4" s="102" t="s">
         <v>160</v>
       </c>
-      <c r="W4" s="103" t="s">
+      <c r="W4" s="102" t="s">
         <v>159</v>
       </c>
-      <c r="X4" s="103" t="s">
+      <c r="X4" s="102" t="s">
         <v>159</v>
       </c>
-      <c r="Y4" s="103" t="s">
+      <c r="Y4" s="102" t="s">
         <v>161</v>
       </c>
-      <c r="Z4" s="103" t="s">
+      <c r="Z4" s="102" t="s">
         <v>162</v>
       </c>
-      <c r="AA4" s="103" t="s">
+      <c r="AA4" s="102" t="s">
         <v>160</v>
       </c>
-      <c r="AB4" s="103" t="s">
+      <c r="AB4" s="102" t="s">
         <v>163</v>
       </c>
-      <c r="AC4" s="103" t="s">
+      <c r="AC4" s="102" t="s">
         <v>164</v>
       </c>
-      <c r="AD4" s="103">
+      <c r="AD4" s="102">
         <v>45</v>
       </c>
-      <c r="AE4" s="110">
+      <c r="AE4" s="109">
         <v>44687</v>
       </c>
-      <c r="AF4" s="110">
+      <c r="AF4" s="109">
         <v>44783</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="15.75" customHeight="1">
-      <c r="A5" s="103" t="s">
+      <c r="A5" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="103" t="s">
+      <c r="B5" s="102" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="103">
+      <c r="D5" s="102">
         <v>15</v>
       </c>
-      <c r="E5" s="103">
+      <c r="E5" s="102">
         <v>74</v>
       </c>
-      <c r="F5" s="103">
+      <c r="F5" s="102">
         <v>99.49</v>
       </c>
-      <c r="G5" s="108">
+      <c r="G5" s="107">
         <f t="shared" si="0"/>
         <v>20.374178581033544</v>
       </c>
-      <c r="H5" s="109">
+      <c r="H5" s="108">
         <f t="shared" si="1"/>
         <v>0.1169316952538656</v>
       </c>
-      <c r="I5" s="108">
+      <c r="I5" s="107">
         <f t="shared" si="2"/>
         <v>53.086989645254981</v>
       </c>
-      <c r="J5" s="103">
+      <c r="J5" s="102">
         <v>1.2</v>
       </c>
-      <c r="K5" s="108">
+      <c r="K5" s="107">
         <f t="shared" si="3"/>
         <v>24.44901429724025</v>
       </c>
-      <c r="M5" s="103"/>
-      <c r="N5" s="103"/>
-      <c r="O5" s="103"/>
-      <c r="P5" s="103"/>
-      <c r="Q5" s="103"/>
-      <c r="R5" s="103"/>
-      <c r="S5" s="103"/>
-      <c r="T5" s="103"/>
-      <c r="U5" s="103"/>
-      <c r="V5" s="103"/>
-      <c r="W5" s="103"/>
-      <c r="X5" s="103"/>
-      <c r="Y5" s="103"/>
-      <c r="Z5" s="103"/>
-      <c r="AA5" s="103"/>
-      <c r="AB5" s="103"/>
-      <c r="AC5" s="103"/>
-      <c r="AD5" s="103"/>
-      <c r="AE5" s="110"/>
-      <c r="AF5" s="110"/>
+      <c r="M5" s="102"/>
+      <c r="N5" s="102"/>
+      <c r="O5" s="102"/>
+      <c r="P5" s="102"/>
+      <c r="Q5" s="102"/>
+      <c r="R5" s="102"/>
+      <c r="S5" s="102"/>
+      <c r="T5" s="102"/>
+      <c r="U5" s="102"/>
+      <c r="V5" s="102"/>
+      <c r="W5" s="102"/>
+      <c r="X5" s="102"/>
+      <c r="Y5" s="102"/>
+      <c r="Z5" s="102"/>
+      <c r="AA5" s="102"/>
+      <c r="AB5" s="102"/>
+      <c r="AC5" s="102"/>
+      <c r="AD5" s="102"/>
+      <c r="AE5" s="109"/>
+      <c r="AF5" s="109"/>
     </row>
     <row r="6" spans="1:35" ht="15.75" customHeight="1">
-      <c r="A6" s="103" t="s">
+      <c r="A6" s="102" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="103" t="s">
+      <c r="B6" s="102" t="s">
         <v>165</v>
       </c>
-      <c r="C6" s="110"/>
-      <c r="D6" s="103">
+      <c r="C6" s="109"/>
+      <c r="D6" s="102">
         <v>15</v>
       </c>
-      <c r="E6" s="103">
+      <c r="E6" s="102">
         <v>88</v>
       </c>
-      <c r="F6" s="103">
+      <c r="F6" s="102">
         <v>99.81</v>
       </c>
-      <c r="G6" s="108">
+      <c r="G6" s="107">
         <f t="shared" si="0"/>
         <v>17.077902560319153</v>
       </c>
-      <c r="H6" s="109">
+      <c r="H6" s="108">
         <f t="shared" si="1"/>
         <v>9.801367401468751E-2</v>
       </c>
-      <c r="I6" s="108">
+      <c r="I6" s="107">
         <f t="shared" si="2"/>
         <v>44.498208002668129</v>
       </c>
-      <c r="J6" s="103">
+      <c r="J6" s="102">
         <v>2.1</v>
       </c>
-      <c r="K6" s="108">
+      <c r="K6" s="107">
         <f t="shared" si="3"/>
         <v>35.863595376670226</v>
       </c>
-      <c r="L6" s="111" t="s">
+      <c r="L6" s="110" t="s">
         <v>166</v>
       </c>
-      <c r="M6" s="103" t="s">
+      <c r="M6" s="102" t="s">
         <v>167</v>
       </c>
-      <c r="N6" s="103">
+      <c r="N6" s="102">
         <v>175000</v>
       </c>
-      <c r="O6" s="103" t="s">
+      <c r="O6" s="102" t="s">
         <v>154</v>
       </c>
-      <c r="P6" s="103" t="s">
+      <c r="P6" s="102" t="s">
         <v>168</v>
       </c>
-      <c r="Q6" s="103" t="s">
+      <c r="Q6" s="102" t="s">
         <v>156</v>
       </c>
-      <c r="R6" s="103">
+      <c r="R6" s="102">
         <v>5</v>
       </c>
-      <c r="S6" s="103" t="s">
+      <c r="S6" s="102" t="s">
         <v>169</v>
       </c>
-      <c r="T6" s="103" t="s">
+      <c r="T6" s="102" t="s">
         <v>158</v>
       </c>
-      <c r="U6" s="103" t="s">
+      <c r="U6" s="102" t="s">
         <v>159</v>
       </c>
-      <c r="V6" s="103" t="s">
+      <c r="V6" s="102" t="s">
         <v>162</v>
       </c>
-      <c r="W6" s="103" t="s">
+      <c r="W6" s="102" t="s">
         <v>170</v>
       </c>
-      <c r="X6" s="103" t="s">
+      <c r="X6" s="102" t="s">
         <v>162</v>
       </c>
-      <c r="Y6" s="103" t="s">
+      <c r="Y6" s="102" t="s">
         <v>170</v>
       </c>
-      <c r="Z6" s="103" t="s">
+      <c r="Z6" s="102" t="s">
         <v>162</v>
       </c>
-      <c r="AA6" s="103" t="s">
+      <c r="AA6" s="102" t="s">
         <v>160</v>
       </c>
-      <c r="AB6" s="103" t="s">
+      <c r="AB6" s="102" t="s">
         <v>163</v>
       </c>
-      <c r="AC6" s="103" t="s">
+      <c r="AC6" s="102" t="s">
         <v>164</v>
       </c>
-      <c r="AD6" s="103">
+      <c r="AD6" s="102">
         <v>40</v>
       </c>
-      <c r="AE6" s="110">
+      <c r="AE6" s="109">
         <v>44720</v>
       </c>
-      <c r="AF6" s="110">
+      <c r="AF6" s="109">
         <v>44849</v>
       </c>
     </row>
     <row r="7" spans="1:35" ht="15.75" customHeight="1">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="102" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="103" t="s">
+      <c r="B7" s="102" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="110"/>
-      <c r="D7" s="103">
+      <c r="C7" s="109"/>
+      <c r="D7" s="102">
         <v>15</v>
       </c>
-      <c r="E7" s="103">
+      <c r="E7" s="102">
         <v>90</v>
       </c>
-      <c r="F7" s="103">
+      <c r="F7" s="102">
         <v>99</v>
       </c>
-      <c r="G7" s="108">
+      <c r="G7" s="107">
         <f t="shared" si="0"/>
         <v>16.835016835016837</v>
       </c>
-      <c r="H7" s="109">
+      <c r="H7" s="108">
         <f t="shared" si="1"/>
         <v>9.6619701762034188E-2</v>
       </c>
-      <c r="I7" s="108">
+      <c r="I7" s="107">
         <f t="shared" si="2"/>
         <v>43.865344599963521</v>
       </c>
-      <c r="J7" s="103">
+      <c r="J7" s="102">
         <v>2.1</v>
       </c>
-      <c r="K7" s="108">
+      <c r="K7" s="107">
         <f t="shared" si="3"/>
         <v>35.353535353535364</v>
       </c>
-      <c r="L7" s="111" t="s">
+      <c r="L7" s="110" t="s">
         <v>171</v>
       </c>
-      <c r="M7" s="103" t="s">
+      <c r="M7" s="102" t="s">
         <v>172</v>
       </c>
-      <c r="N7" s="103">
+      <c r="N7" s="102">
         <v>100000</v>
       </c>
-      <c r="O7" s="103" t="s">
+      <c r="O7" s="102" t="s">
         <v>154</v>
       </c>
-      <c r="P7" s="103" t="s">
+      <c r="P7" s="102" t="s">
         <v>155</v>
       </c>
-      <c r="Q7" s="103" t="s">
+      <c r="Q7" s="102" t="s">
         <v>156</v>
       </c>
-      <c r="R7" s="103">
+      <c r="R7" s="102">
         <v>25</v>
       </c>
-      <c r="S7" s="103" t="s">
+      <c r="S7" s="102" t="s">
         <v>173</v>
       </c>
-      <c r="T7" s="103" t="s">
+      <c r="T7" s="102" t="s">
         <v>158</v>
       </c>
-      <c r="U7" s="103" t="s">
+      <c r="U7" s="102" t="s">
         <v>159</v>
       </c>
-      <c r="V7" s="103" t="s">
+      <c r="V7" s="102" t="s">
         <v>170</v>
       </c>
-      <c r="W7" s="103" t="s">
+      <c r="W7" s="102" t="s">
         <v>161</v>
       </c>
-      <c r="X7" s="103" t="s">
+      <c r="X7" s="102" t="s">
         <v>170</v>
       </c>
-      <c r="Y7" s="103" t="s">
+      <c r="Y7" s="102" t="s">
         <v>161</v>
       </c>
-      <c r="Z7" s="103" t="s">
+      <c r="Z7" s="102" t="s">
         <v>160</v>
       </c>
-      <c r="AA7" s="103" t="s">
+      <c r="AA7" s="102" t="s">
         <v>160</v>
       </c>
-      <c r="AB7" s="103" t="s">
+      <c r="AB7" s="102" t="s">
         <v>163</v>
       </c>
-      <c r="AC7" s="103" t="s">
+      <c r="AC7" s="102" t="s">
         <v>174</v>
       </c>
-      <c r="AD7" s="103">
+      <c r="AD7" s="102">
         <v>40</v>
       </c>
-      <c r="AE7" s="110">
+      <c r="AE7" s="109">
         <v>44720</v>
       </c>
-      <c r="AF7" s="110">
+      <c r="AF7" s="109">
         <v>44849</v>
       </c>
     </row>
     <row r="8" spans="1:35" ht="15.75" customHeight="1">
-      <c r="A8" s="103" t="s">
+      <c r="A8" s="102" t="s">
         <v>175</v>
       </c>
-      <c r="B8" s="103" t="s">
+      <c r="B8" s="102" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="103">
+      <c r="D8" s="102">
         <v>15</v>
       </c>
-      <c r="E8" s="103">
+      <c r="E8" s="102">
         <v>83</v>
       </c>
-      <c r="F8" s="103">
+      <c r="F8" s="102">
         <v>99.95</v>
       </c>
-      <c r="G8" s="108">
+      <c r="G8" s="107">
         <f t="shared" si="0"/>
         <v>18.081329821537274</v>
       </c>
-      <c r="H8" s="109">
+      <c r="H8" s="108">
         <f t="shared" si="1"/>
         <v>0.10377255407218361</v>
       </c>
-      <c r="I8" s="108">
+      <c r="I8" s="107">
         <f t="shared" si="2"/>
         <v>47.112739548771358</v>
       </c>
-      <c r="J8" s="103">
+      <c r="J8" s="102">
         <v>2.25</v>
       </c>
-      <c r="K8" s="108">
+      <c r="K8" s="107">
         <f t="shared" si="3"/>
         <v>40.682992098458868</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="15.75" customHeight="1">
-      <c r="A9" s="103" t="s">
+      <c r="A9" s="102" t="s">
         <v>79</v>
       </c>
-      <c r="B9" s="103" t="s">
+      <c r="B9" s="102" t="s">
         <v>176</v>
       </c>
-      <c r="C9" s="110"/>
-      <c r="D9" s="103">
+      <c r="C9" s="109"/>
+      <c r="D9" s="102">
         <v>15</v>
       </c>
-      <c r="E9" s="103">
+      <c r="E9" s="102">
         <v>94</v>
       </c>
-      <c r="F9" s="103">
+      <c r="F9" s="102">
         <v>99.9</v>
       </c>
-      <c r="G9" s="108">
+      <c r="G9" s="107">
         <f t="shared" si="0"/>
         <v>15.973420228739377</v>
       </c>
-      <c r="H9" s="109">
+      <c r="H9" s="108">
         <f t="shared" si="1"/>
         <v>9.167481765805427E-2</v>
       </c>
-      <c r="I9" s="108">
+      <c r="I9" s="107">
         <f t="shared" si="2"/>
         <v>41.620367216756641</v>
       </c>
-      <c r="J9" s="103">
+      <c r="J9" s="102">
         <v>2.25</v>
       </c>
-      <c r="K9" s="108">
+      <c r="K9" s="107">
         <f t="shared" si="3"/>
         <v>35.9401955146636</v>
       </c>
-      <c r="L9" s="111" t="s">
+      <c r="L9" s="110" t="s">
         <v>177</v>
       </c>
-      <c r="M9" s="103" t="s">
+      <c r="M9" s="102" t="s">
         <v>178</v>
       </c>
-      <c r="N9" s="103">
+      <c r="N9" s="102">
         <v>100000</v>
       </c>
-      <c r="O9" s="103" t="s">
+      <c r="O9" s="102" t="s">
         <v>154</v>
       </c>
-      <c r="P9" s="103" t="s">
+      <c r="P9" s="102" t="s">
         <v>155</v>
       </c>
-      <c r="Q9" s="103" t="s">
+      <c r="Q9" s="102" t="s">
         <v>156</v>
       </c>
-      <c r="R9" s="103">
+      <c r="R9" s="102">
         <v>25</v>
       </c>
-      <c r="S9" s="103" t="s">
+      <c r="S9" s="102" t="s">
         <v>179</v>
       </c>
-      <c r="T9" s="103" t="s">
+      <c r="T9" s="102" t="s">
         <v>158</v>
       </c>
-      <c r="U9" s="103" t="s">
+      <c r="U9" s="102" t="s">
         <v>159</v>
       </c>
-      <c r="V9" s="103" t="s">
+      <c r="V9" s="102" t="s">
         <v>170</v>
       </c>
-      <c r="W9" s="103" t="s">
+      <c r="W9" s="102" t="s">
         <v>161</v>
       </c>
-      <c r="X9" s="103" t="s">
+      <c r="X9" s="102" t="s">
         <v>161</v>
       </c>
-      <c r="Y9" s="103" t="s">
+      <c r="Y9" s="102" t="s">
         <v>161</v>
       </c>
-      <c r="Z9" s="103" t="s">
+      <c r="Z9" s="102" t="s">
         <v>160</v>
       </c>
-      <c r="AA9" s="103" t="s">
+      <c r="AA9" s="102" t="s">
         <v>160</v>
       </c>
-      <c r="AB9" s="103" t="s">
+      <c r="AB9" s="102" t="s">
         <v>180</v>
       </c>
-      <c r="AC9" s="103" t="s">
+      <c r="AC9" s="102" t="s">
         <v>181</v>
       </c>
-      <c r="AD9" s="103">
+      <c r="AD9" s="102">
         <v>40</v>
       </c>
-      <c r="AE9" s="110">
+      <c r="AE9" s="109">
         <v>44720</v>
       </c>
-      <c r="AF9" s="110">
+      <c r="AF9" s="109">
         <v>44849</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="15.75" customHeight="1">
-      <c r="A10" s="103" t="s">
+      <c r="A10" s="102" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="103" t="s">
+      <c r="B10" s="102" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="103">
+      <c r="D10" s="102">
         <v>15</v>
       </c>
-      <c r="E10" s="103">
+      <c r="E10" s="102">
         <v>95</v>
       </c>
-      <c r="F10" s="103">
+      <c r="F10" s="102">
         <v>98.82</v>
       </c>
-      <c r="G10" s="108">
+      <c r="G10" s="107">
         <f t="shared" si="0"/>
         <v>15.978014252388714</v>
       </c>
-      <c r="H10" s="109">
+      <c r="H10" s="108">
         <f t="shared" si="1"/>
         <v>9.170118372583054E-2</v>
       </c>
-      <c r="I10" s="108">
+      <c r="I10" s="107">
         <f t="shared" si="2"/>
         <v>41.632337411527068</v>
       </c>
-      <c r="J10" s="103">
+      <c r="J10" s="102">
         <v>2.25</v>
       </c>
-      <c r="K10" s="108">
+      <c r="K10" s="107">
         <f t="shared" si="3"/>
         <v>35.950532067874605</v>
       </c>
-      <c r="M10" s="112"/>
+      <c r="M10" s="111"/>
     </row>
     <row r="11" spans="1:35" ht="15.75" customHeight="1">
-      <c r="A11" s="103" t="s">
+      <c r="A11" s="102" t="s">
         <v>183</v>
       </c>
-      <c r="B11" s="103" t="s">
+      <c r="B11" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="D11" s="103">
+      <c r="D11" s="102">
         <v>8</v>
       </c>
-      <c r="E11" s="103">
+      <c r="E11" s="102">
         <v>95</v>
       </c>
-      <c r="F11" s="103">
+      <c r="F11" s="102">
         <v>99.76</v>
       </c>
-      <c r="G11" s="108">
+      <c r="G11" s="107">
         <f t="shared" si="0"/>
         <v>8.4413117798505883</v>
       </c>
-      <c r="H11" s="109">
+      <c r="H11" s="108">
         <f t="shared" si="1"/>
         <v>4.8446463382980878E-2</v>
       </c>
-      <c r="I11" s="108">
+      <c r="I11" s="107">
         <f t="shared" si="2"/>
         <v>21.994694375873319</v>
       </c>
-      <c r="J11" s="103">
+      <c r="J11" s="102">
         <v>2.95</v>
       </c>
-      <c r="K11" s="108">
+      <c r="K11" s="107">
         <f t="shared" si="3"/>
         <v>24.901869750559236</v>
       </c>
-      <c r="N11" s="103">
+      <c r="N11" s="102">
         <v>280000</v>
       </c>
     </row>
     <row r="12" spans="1:35" ht="15.75" customHeight="1">
-      <c r="A12" s="103" t="s">
+      <c r="A12" s="102" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="103" t="s">
+      <c r="B12" s="102" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="103">
+      <c r="D12" s="102">
         <v>10</v>
       </c>
-      <c r="E12" s="103">
+      <c r="E12" s="102">
         <v>73</v>
       </c>
-      <c r="F12" s="103">
+      <c r="F12" s="102">
         <v>99.51</v>
       </c>
-      <c r="G12" s="108">
+      <c r="G12" s="107">
         <f t="shared" si="0"/>
         <v>13.766083948333131</v>
       </c>
-      <c r="H12" s="109">
+      <c r="H12" s="108">
         <f t="shared" si="1"/>
         <v>7.9006450575832929E-2</v>
       </c>
-      <c r="I12" s="108">
+      <c r="I12" s="107">
         <f t="shared" si="2"/>
         <v>35.868928561428149</v>
       </c>
-      <c r="J12" s="103">
+      <c r="J12" s="102">
         <v>1.9</v>
       </c>
-      <c r="K12" s="108">
+      <c r="K12" s="107">
         <f t="shared" si="3"/>
         <v>26.155559501832947</v>
       </c>
-      <c r="N12" s="103">
+      <c r="N12" s="102">
         <f>1000/(1/454)</f>
         <v>453999.99999999994</v>
       </c>
     </row>
     <row r="13" spans="1:35" ht="15.75" customHeight="1">
-      <c r="A13" s="113" t="s">
+      <c r="A13" s="112" t="s">
         <v>184</v>
       </c>
-      <c r="B13" s="103" t="s">
+      <c r="B13" s="102" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="103">
+      <c r="D13" s="102">
         <v>10</v>
       </c>
-      <c r="E13" s="103">
+      <c r="E13" s="102">
         <v>95</v>
       </c>
-      <c r="F13" s="103">
+      <c r="F13" s="102">
         <v>99.79</v>
       </c>
-      <c r="G13" s="108">
+      <c r="G13" s="107">
         <f t="shared" si="0"/>
         <v>10.548467571373569</v>
       </c>
-      <c r="H13" s="109">
+      <c r="H13" s="108">
         <f t="shared" si="1"/>
         <v>6.0539873573080626E-2</v>
       </c>
-      <c r="I13" s="108">
+      <c r="I13" s="107">
         <f t="shared" si="2"/>
         <v>27.485102602178603</v>
       </c>
-      <c r="J13" s="103">
+      <c r="J13" s="102">
         <v>2.5</v>
       </c>
-      <c r="K13" s="108">
+      <c r="K13" s="107">
         <f t="shared" si="3"/>
         <v>26.371168928433924</v>
       </c>
-      <c r="N13" s="103">
+      <c r="N13" s="102">
         <f>600/(2/454)</f>
         <v>136200</v>
       </c>
     </row>
     <row r="14" spans="1:35" ht="15.75" customHeight="1">
-      <c r="A14" s="114" t="s">
+      <c r="A14" s="113" t="s">
         <v>185</v>
       </c>
-      <c r="B14" s="114" t="s">
+      <c r="B14" s="113" t="s">
         <v>186</v>
       </c>
-      <c r="C14" s="115"/>
-      <c r="D14" s="114">
+      <c r="C14" s="114"/>
+      <c r="D14" s="113">
         <v>10</v>
       </c>
-      <c r="E14" s="114"/>
-      <c r="F14" s="114"/>
-      <c r="G14" s="108" t="e">
+      <c r="E14" s="113"/>
+      <c r="F14" s="113"/>
+      <c r="G14" s="107" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H14" s="109" t="e">
+      <c r="H14" s="108" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I14" s="108" t="e">
+      <c r="I14" s="107" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J14" s="114"/>
-      <c r="K14" s="114"/>
-      <c r="L14" s="116" t="s">
+      <c r="J14" s="113"/>
+      <c r="K14" s="113"/>
+      <c r="L14" s="115" t="s">
         <v>187</v>
       </c>
-      <c r="M14" s="114" t="s">
+      <c r="M14" s="113" t="s">
         <v>172</v>
       </c>
-      <c r="N14" s="114">
+      <c r="N14" s="113">
         <v>180000</v>
       </c>
-      <c r="O14" s="114" t="s">
+      <c r="O14" s="113" t="s">
         <v>154</v>
       </c>
-      <c r="P14" s="114" t="s">
+      <c r="P14" s="113" t="s">
         <v>155</v>
       </c>
-      <c r="Q14" s="114" t="s">
+      <c r="Q14" s="113" t="s">
         <v>156</v>
       </c>
-      <c r="R14" s="114">
+      <c r="R14" s="113">
         <v>15</v>
       </c>
-      <c r="S14" s="114" t="s">
+      <c r="S14" s="113" t="s">
         <v>157</v>
       </c>
-      <c r="T14" s="114" t="s">
+      <c r="T14" s="113" t="s">
         <v>158</v>
       </c>
-      <c r="U14" s="114" t="s">
+      <c r="U14" s="113" t="s">
         <v>170</v>
       </c>
-      <c r="V14" s="114" t="s">
+      <c r="V14" s="113" t="s">
         <v>162</v>
       </c>
-      <c r="W14" s="114" t="s">
+      <c r="W14" s="113" t="s">
         <v>161</v>
       </c>
-      <c r="X14" s="114" t="s">
+      <c r="X14" s="113" t="s">
         <v>161</v>
       </c>
-      <c r="Y14" s="114" t="s">
+      <c r="Y14" s="113" t="s">
         <v>170</v>
       </c>
-      <c r="Z14" s="114" t="s">
+      <c r="Z14" s="113" t="s">
         <v>160</v>
       </c>
-      <c r="AA14" s="114" t="s">
+      <c r="AA14" s="113" t="s">
         <v>160</v>
       </c>
-      <c r="AB14" s="114" t="s">
+      <c r="AB14" s="113" t="s">
         <v>180</v>
       </c>
-      <c r="AC14" s="114" t="s">
+      <c r="AC14" s="113" t="s">
         <v>164</v>
       </c>
-      <c r="AD14" s="114">
+      <c r="AD14" s="113">
         <v>42</v>
       </c>
-      <c r="AE14" s="115">
+      <c r="AE14" s="114">
         <v>44687</v>
       </c>
-      <c r="AF14" s="115">
+      <c r="AF14" s="114">
         <v>44783</v>
       </c>
-      <c r="AG14" s="114"/>
-      <c r="AH14" s="114"/>
-      <c r="AI14" s="114"/>
+      <c r="AG14" s="113"/>
+      <c r="AH14" s="113"/>
+      <c r="AI14" s="113"/>
     </row>
     <row r="15" spans="1:35" ht="15.75" customHeight="1">
-      <c r="A15" s="114" t="s">
+      <c r="A15" s="113" t="s">
         <v>188</v>
       </c>
-      <c r="B15" s="114" t="s">
+      <c r="B15" s="113" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="115"/>
-      <c r="D15" s="114">
+      <c r="C15" s="114"/>
+      <c r="D15" s="113">
         <v>10</v>
       </c>
-      <c r="E15" s="114"/>
-      <c r="F15" s="114"/>
-      <c r="G15" s="108" t="e">
+      <c r="E15" s="113"/>
+      <c r="F15" s="113"/>
+      <c r="G15" s="107" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H15" s="109" t="e">
+      <c r="H15" s="108" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I15" s="108" t="e">
+      <c r="I15" s="107" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J15" s="114"/>
-      <c r="K15" s="114"/>
-      <c r="L15" s="116" t="s">
+      <c r="J15" s="113"/>
+      <c r="K15" s="113"/>
+      <c r="L15" s="115" t="s">
         <v>189</v>
       </c>
-      <c r="M15" s="114" t="s">
+      <c r="M15" s="113" t="s">
         <v>153</v>
       </c>
-      <c r="N15" s="114">
+      <c r="N15" s="113">
         <v>175000</v>
       </c>
-      <c r="O15" s="114" t="s">
+      <c r="O15" s="113" t="s">
         <v>154</v>
       </c>
-      <c r="P15" s="114" t="s">
+      <c r="P15" s="113" t="s">
         <v>155</v>
       </c>
-      <c r="Q15" s="114" t="s">
+      <c r="Q15" s="113" t="s">
         <v>156</v>
       </c>
-      <c r="R15" s="114">
+      <c r="R15" s="113">
         <v>0</v>
       </c>
-      <c r="S15" s="114" t="s">
+      <c r="S15" s="113" t="s">
         <v>190</v>
       </c>
-      <c r="T15" s="114" t="s">
+      <c r="T15" s="113" t="s">
         <v>158</v>
       </c>
-      <c r="U15" s="114" t="s">
+      <c r="U15" s="113" t="s">
         <v>159</v>
       </c>
-      <c r="V15" s="114" t="s">
+      <c r="V15" s="113" t="s">
         <v>160</v>
       </c>
-      <c r="W15" s="114" t="s">
+      <c r="W15" s="113" t="s">
         <v>161</v>
       </c>
-      <c r="X15" s="114" t="s">
+      <c r="X15" s="113" t="s">
         <v>170</v>
       </c>
-      <c r="Y15" s="114" t="s">
+      <c r="Y15" s="113" t="s">
         <v>170</v>
       </c>
-      <c r="Z15" s="114" t="s">
+      <c r="Z15" s="113" t="s">
         <v>160</v>
       </c>
-      <c r="AA15" s="114" t="s">
+      <c r="AA15" s="113" t="s">
         <v>170</v>
       </c>
-      <c r="AB15" s="114" t="s">
+      <c r="AB15" s="113" t="s">
         <v>163</v>
       </c>
-      <c r="AC15" s="114" t="s">
+      <c r="AC15" s="113" t="s">
         <v>164</v>
       </c>
-      <c r="AD15" s="114">
+      <c r="AD15" s="113">
         <v>43</v>
       </c>
-      <c r="AE15" s="115">
+      <c r="AE15" s="114">
         <v>44687</v>
       </c>
-      <c r="AF15" s="115">
+      <c r="AF15" s="114">
         <v>44783</v>
       </c>
-      <c r="AG15" s="114"/>
-      <c r="AH15" s="114"/>
-      <c r="AI15" s="114"/>
+      <c r="AG15" s="113"/>
+      <c r="AH15" s="113"/>
+      <c r="AI15" s="113"/>
     </row>
     <row r="16" spans="1:35" ht="15.75" customHeight="1">
-      <c r="A16" s="103" t="s">
+      <c r="A16" s="102" t="s">
         <v>98</v>
       </c>
-      <c r="B16" s="103" t="s">
+      <c r="B16" s="102" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="103">
+      <c r="D16" s="102">
         <v>12</v>
       </c>
-      <c r="E16" s="103">
+      <c r="E16" s="102">
         <v>78</v>
       </c>
-      <c r="F16" s="103">
+      <c r="F16" s="102">
         <v>64</v>
       </c>
-      <c r="G16" s="108">
+      <c r="G16" s="107">
         <f t="shared" si="0"/>
         <v>24.038461538461537</v>
       </c>
-      <c r="H16" s="109">
+      <c r="H16" s="108">
         <f t="shared" si="1"/>
         <v>0.1379617856890584</v>
       </c>
-      <c r="I16" s="108">
+      <c r="I16" s="107">
         <f t="shared" si="2"/>
         <v>62.634650702832509</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A17" s="103" t="s">
+      <c r="A17" s="102" t="s">
         <v>102</v>
       </c>
-      <c r="B17" s="103" t="s">
+      <c r="B17" s="102" t="s">
         <v>103</v>
       </c>
-      <c r="D17" s="103">
+      <c r="D17" s="102">
         <v>20</v>
       </c>
-      <c r="E17" s="103">
+      <c r="E17" s="102">
         <v>99.6</v>
       </c>
-      <c r="F17" s="103">
+      <c r="F17" s="102">
         <v>68</v>
       </c>
-      <c r="G17" s="108">
+      <c r="G17" s="107">
         <f t="shared" si="0"/>
         <v>29.529884242853768</v>
       </c>
-      <c r="H17" s="109">
+      <c r="H17" s="108">
         <f t="shared" si="1"/>
         <v>0.16947821535154825</v>
       </c>
-      <c r="I17" s="108">
+      <c r="I17" s="107">
         <f t="shared" si="2"/>
         <v>76.943109769602913</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1">
-      <c r="G18" s="103">
+      <c r="G18" s="102">
         <f>(1/20)*43560</f>
         <v>2178</v>
       </c>
-      <c r="J18" s="103">
+      <c r="J18" s="102">
         <f>G18/8</f>
         <v>272.25</v>
       </c>
-      <c r="K18" s="103">
+      <c r="K18" s="102">
         <f>J18/25</f>
         <v>10.89</v>
       </c>
@@ -5288,332 +5324,332 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A1" s="117"/>
-      <c r="B1" s="118" t="s">
+      <c r="A1" s="116"/>
+      <c r="B1" s="117" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="118" t="s">
+      <c r="C1" s="117" t="s">
         <v>191</v>
       </c>
-      <c r="D1" s="118" t="s">
+      <c r="D1" s="117" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="118" t="s">
+      <c r="E1" s="117" t="s">
         <v>192</v>
       </c>
-      <c r="F1" s="119" t="s">
+      <c r="F1" s="118" t="s">
         <v>127</v>
       </c>
-      <c r="G1" s="120" t="s">
+      <c r="G1" s="119" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="120" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="122" t="s">
+      <c r="B2" s="121" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="122" t="s">
+      <c r="C2" s="121" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="123">
+      <c r="D2" s="122">
         <v>15</v>
       </c>
-      <c r="E2" s="124">
+      <c r="E2" s="123">
         <v>16.218232537018114</v>
       </c>
-      <c r="F2" s="125">
+      <c r="F2" s="124">
         <v>30.814641820334415</v>
       </c>
-      <c r="G2" s="126">
+      <c r="G2" s="125">
         <v>42.258250526895218</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="120" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="122" t="s">
+      <c r="B3" s="121" t="s">
         <v>150</v>
       </c>
-      <c r="C3" s="122" t="s">
+      <c r="C3" s="121" t="s">
         <v>151</v>
       </c>
-      <c r="D3" s="123">
+      <c r="D3" s="122">
         <v>10</v>
       </c>
-      <c r="E3" s="124">
+      <c r="E3" s="123">
         <v>10.644684683150317</v>
       </c>
-      <c r="F3" s="125">
+      <c r="F3" s="124">
         <v>18.628198195513054</v>
       </c>
-      <c r="G3" s="126">
+      <c r="G3" s="125">
         <v>27.735806049989918</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="122" t="s">
+      <c r="B4" s="121" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="122" t="s">
+      <c r="C4" s="121" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="123">
+      <c r="D4" s="122">
         <v>15</v>
       </c>
-      <c r="E4" s="124">
+      <c r="E4" s="123">
         <v>20.374178581033544</v>
       </c>
-      <c r="F4" s="125">
+      <c r="F4" s="124">
         <v>24.44901429724025</v>
       </c>
-      <c r="G4" s="126">
+      <c r="G4" s="125">
         <v>53.086989645254981</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A5" s="121" t="s">
+      <c r="A5" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="122" t="s">
+      <c r="B5" s="121" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="122" t="s">
+      <c r="C5" s="121" t="s">
         <v>165</v>
       </c>
-      <c r="D5" s="123">
+      <c r="D5" s="122">
         <v>15</v>
       </c>
-      <c r="E5" s="124">
+      <c r="E5" s="123">
         <v>17.077902560319153</v>
       </c>
-      <c r="F5" s="125">
+      <c r="F5" s="124">
         <v>35.863595376670226</v>
       </c>
-      <c r="G5" s="126">
+      <c r="G5" s="125">
         <v>44.498208002668129</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A6" s="121" t="s">
+      <c r="A6" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="122" t="s">
+      <c r="B6" s="121" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="122" t="s">
+      <c r="C6" s="121" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="123">
+      <c r="D6" s="122">
         <v>15</v>
       </c>
-      <c r="E6" s="124">
+      <c r="E6" s="123">
         <v>16.835016835016837</v>
       </c>
-      <c r="F6" s="125">
+      <c r="F6" s="124">
         <v>35.353535353535364</v>
       </c>
-      <c r="G6" s="126">
+      <c r="G6" s="125">
         <v>43.865344599963521</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A7" s="121" t="s">
+      <c r="A7" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="122" t="s">
+      <c r="B7" s="121" t="s">
         <v>175</v>
       </c>
-      <c r="C7" s="122" t="s">
+      <c r="C7" s="121" t="s">
         <v>76</v>
       </c>
-      <c r="D7" s="123">
+      <c r="D7" s="122">
         <v>15</v>
       </c>
-      <c r="E7" s="124">
+      <c r="E7" s="123">
         <v>18.081329821537274</v>
       </c>
-      <c r="F7" s="125">
+      <c r="F7" s="124">
         <v>40.682992098458868</v>
       </c>
-      <c r="G7" s="126">
+      <c r="G7" s="125">
         <v>47.112739548771358</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A8" s="121" t="s">
+      <c r="A8" s="120" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="122" t="s">
+      <c r="B8" s="121" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="122" t="s">
+      <c r="C8" s="121" t="s">
         <v>176</v>
       </c>
-      <c r="D8" s="123">
+      <c r="D8" s="122">
         <v>15</v>
       </c>
-      <c r="E8" s="124">
+      <c r="E8" s="123">
         <v>15.973420228739377</v>
       </c>
-      <c r="F8" s="125">
+      <c r="F8" s="124">
         <v>35.9401955146636</v>
       </c>
-      <c r="G8" s="126">
+      <c r="G8" s="125">
         <v>41.620367216756641</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A9" s="121" t="s">
+      <c r="A9" s="120" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="122" t="s">
+      <c r="B9" s="121" t="s">
         <v>182</v>
       </c>
-      <c r="C9" s="122" t="s">
+      <c r="C9" s="121" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="123">
+      <c r="D9" s="122">
         <v>15</v>
       </c>
-      <c r="E9" s="124">
+      <c r="E9" s="123">
         <v>15.978014252388714</v>
       </c>
-      <c r="F9" s="125">
+      <c r="F9" s="124">
         <v>35.950532067874605</v>
       </c>
-      <c r="G9" s="126">
+      <c r="G9" s="125">
         <v>41.632337411527068</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A10" s="121" t="s">
+      <c r="A10" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="122" t="s">
+      <c r="B10" s="121" t="s">
         <v>183</v>
       </c>
-      <c r="C10" s="122" t="s">
+      <c r="C10" s="121" t="s">
         <v>87</v>
       </c>
-      <c r="D10" s="123">
+      <c r="D10" s="122">
         <v>8</v>
       </c>
-      <c r="E10" s="124">
+      <c r="E10" s="123">
         <v>8.4413117798505883</v>
       </c>
-      <c r="F10" s="125">
+      <c r="F10" s="124">
         <v>24.901869750559236</v>
       </c>
-      <c r="G10" s="126">
+      <c r="G10" s="125">
         <v>21.994694375873319</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A11" s="121" t="s">
+      <c r="A11" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="122" t="s">
+      <c r="B11" s="121" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="122" t="s">
+      <c r="C11" s="121" t="s">
         <v>91</v>
       </c>
-      <c r="D11" s="123">
+      <c r="D11" s="122">
         <v>10</v>
       </c>
-      <c r="E11" s="124">
+      <c r="E11" s="123">
         <v>13.766083948333131</v>
       </c>
-      <c r="F11" s="125">
+      <c r="F11" s="124">
         <v>26.155559501832947</v>
       </c>
-      <c r="G11" s="126">
+      <c r="G11" s="125">
         <v>35.868928561428149</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A12" s="121" t="s">
+      <c r="A12" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="127" t="s">
+      <c r="B12" s="126" t="s">
         <v>94</v>
       </c>
-      <c r="C12" s="122" t="s">
+      <c r="C12" s="121" t="s">
         <v>95</v>
       </c>
-      <c r="D12" s="123">
+      <c r="D12" s="122">
         <v>10</v>
       </c>
-      <c r="E12" s="124">
+      <c r="E12" s="123">
         <v>10.548467571373569</v>
       </c>
-      <c r="F12" s="125">
+      <c r="F12" s="124">
         <v>26.371168928433924</v>
       </c>
-      <c r="G12" s="126">
+      <c r="G12" s="125">
         <v>27.485102602178603</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A13" s="121" t="s">
+      <c r="A13" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="128" t="s">
+      <c r="B13" s="127" t="s">
         <v>98</v>
       </c>
-      <c r="C13" s="122" t="s">
+      <c r="C13" s="121" t="s">
         <v>99</v>
       </c>
-      <c r="D13" s="122">
+      <c r="D13" s="121">
         <v>12</v>
       </c>
-      <c r="E13" s="125">
+      <c r="E13" s="124">
         <v>24.038461538461537</v>
       </c>
-      <c r="F13" s="122"/>
-      <c r="G13" s="129">
+      <c r="F13" s="121"/>
+      <c r="G13" s="128">
         <v>62.634650702832509</v>
       </c>
-      <c r="H13" s="108"/>
-      <c r="I13" s="109"/>
-      <c r="J13" s="108"/>
+      <c r="H13" s="107"/>
+      <c r="I13" s="108"/>
+      <c r="J13" s="107"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A14" s="121" t="s">
+      <c r="A14" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="128" t="s">
+      <c r="B14" s="127" t="s">
         <v>102</v>
       </c>
-      <c r="C14" s="122" t="s">
+      <c r="C14" s="121" t="s">
         <v>103</v>
       </c>
-      <c r="D14" s="122">
+      <c r="D14" s="121">
         <v>20</v>
       </c>
-      <c r="E14" s="125">
+      <c r="E14" s="124">
         <v>29.529884242853768</v>
       </c>
-      <c r="F14" s="122"/>
-      <c r="G14" s="129">
+      <c r="F14" s="121"/>
+      <c r="G14" s="128">
         <v>76.943109769602913</v>
       </c>
-      <c r="H14" s="108"/>
-      <c r="I14" s="109"/>
-      <c r="J14" s="108"/>
+      <c r="H14" s="107"/>
+      <c r="I14" s="108"/>
+      <c r="J14" s="107"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1">
-      <c r="H16" s="108"/>
+      <c r="H16" s="107"/>
     </row>
     <row r="17" spans="8:8" ht="15.75" customHeight="1">
-      <c r="H17" s="108"/>
+      <c r="H17" s="107"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5632,10 +5668,10 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="110" t="s">
         <v>194</v>
       </c>
-      <c r="B1" s="103" t="s">
+      <c r="B1" s="102" t="s">
         <v>195</v>
       </c>
     </row>
@@ -5655,7 +5691,7 @@
   </sheetPr>
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
@@ -5670,95 +5706,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="102" t="s">
         <v>196</v>
       </c>
-      <c r="C1" s="103" t="s">
+      <c r="C1" s="102" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="102" t="s">
         <v>198</v>
       </c>
-      <c r="C2" s="103" t="s">
+      <c r="C2" s="102" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A3" s="103" t="s">
+      <c r="A3" s="102" t="s">
         <v>199</v>
       </c>
-      <c r="C3" s="103" t="s">
+      <c r="C3" s="102" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="103" t="s">
+      <c r="C4" s="102" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A5" s="103" t="s">
+      <c r="A5" s="102" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A6" s="103" t="s">
+      <c r="A6" s="102" t="s">
         <v>201</v>
       </c>
-      <c r="C6" s="103" t="s">
+      <c r="C6" s="102" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="102" t="s">
         <v>203</v>
       </c>
-      <c r="C7" s="103" t="s">
+      <c r="C7" s="102" t="s">
         <v>204</v>
       </c>
-      <c r="J7" s="130"/>
-      <c r="K7" s="130"/>
-      <c r="L7" s="130"/>
-      <c r="M7" s="130"/>
+      <c r="J7" s="129"/>
+      <c r="K7" s="129"/>
+      <c r="L7" s="129"/>
+      <c r="M7" s="129"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A8" s="103" t="s">
+      <c r="A8" s="102" t="s">
         <v>205</v>
       </c>
-      <c r="C8" s="103">
+      <c r="C8" s="102">
         <v>4010</v>
       </c>
-      <c r="I8" s="131"/>
-      <c r="J8" s="146"/>
-      <c r="K8" s="147"/>
-      <c r="L8" s="147"/>
-      <c r="M8" s="148"/>
+      <c r="I8" s="130"/>
+      <c r="J8" s="145"/>
+      <c r="K8" s="146"/>
+      <c r="L8" s="146"/>
+      <c r="M8" s="147"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1">
-      <c r="I9" s="130"/>
-      <c r="J9" s="132"/>
-      <c r="K9" s="132"/>
-      <c r="L9" s="132"/>
-      <c r="M9" s="132"/>
+      <c r="I9" s="129"/>
+      <c r="J9" s="131"/>
+      <c r="K9" s="131"/>
+      <c r="L9" s="131"/>
+      <c r="M9" s="131"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1">
-      <c r="I10" s="130"/>
-      <c r="J10" s="132"/>
-      <c r="K10" s="132"/>
-      <c r="L10" s="132"/>
-      <c r="M10" s="132"/>
+      <c r="I10" s="129"/>
+      <c r="J10" s="131"/>
+      <c r="K10" s="131"/>
+      <c r="L10" s="131"/>
+      <c r="M10" s="131"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1">
-      <c r="I11" s="130"/>
-      <c r="J11" s="132"/>
-      <c r="K11" s="132"/>
-      <c r="L11" s="132"/>
-      <c r="M11" s="132"/>
+      <c r="I11" s="129"/>
+      <c r="J11" s="131"/>
+      <c r="K11" s="131"/>
+      <c r="L11" s="131"/>
+      <c r="M11" s="131"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>